<commit_message>
Added REST API to orchestrator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -141,9 +141,6 @@
     <t>QueueName</t>
   </si>
   <si>
-    <t>ProcessQueue</t>
-  </si>
-  <si>
     <t>Orchestrator Queue Name. Be sure to match the two names.</t>
   </si>
   <si>
@@ -154,12 +151,45 @@
   </si>
   <si>
     <t>System exception.</t>
+  </si>
+  <si>
+    <t>Orch_tenancyName</t>
+  </si>
+  <si>
+    <t>fantastic</t>
+  </si>
+  <si>
+    <t>Orch_env</t>
+  </si>
+  <si>
+    <t>mihhdusENV</t>
+  </si>
+  <si>
+    <t>Orch_orchestratorURL</t>
+  </si>
+  <si>
+    <t>https://demo.uipath.com</t>
+  </si>
+  <si>
+    <t>Orch_userNameOrEmailAddress</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Orch_password</t>
+  </si>
+  <si>
+    <t>123qwe</t>
+  </si>
+  <si>
+    <t>KibanaDemoQueue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -537,11 +567,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,10 +597,50 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
-        <v>42</v>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -580,11 +650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +823,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -764,7 +834,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -775,7 +845,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -788,7 +858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
orchestrator credentials are now stored in WCM
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -138,12 +138,6 @@
     <t>AccuracyHigh</t>
   </si>
   <si>
-    <t>QueueName</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match the two names.</t>
-  </si>
-  <si>
     <t>Transaction Successful.</t>
   </si>
   <si>
@@ -153,37 +147,40 @@
     <t>System exception.</t>
   </si>
   <si>
-    <t>Orch_tenancyName</t>
-  </si>
-  <si>
     <t>fantastic</t>
   </si>
   <si>
-    <t>Orch_env</t>
-  </si>
-  <si>
-    <t>mihhdusENV</t>
-  </si>
-  <si>
-    <t>Orch_orchestratorURL</t>
-  </si>
-  <si>
     <t>https://demo.uipath.com</t>
   </si>
   <si>
-    <t>Orch_userNameOrEmailAddress</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Orch_password</t>
-  </si>
-  <si>
-    <t>123qwe</t>
-  </si>
-  <si>
     <t>KibanaDemoQueue</t>
+  </si>
+  <si>
+    <t>demo.uipath.com_credentials</t>
+  </si>
+  <si>
+    <t>OrchestratorURL</t>
+  </si>
+  <si>
+    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
+  </si>
+  <si>
+    <t>OrchestratorCredentialName</t>
+  </si>
+  <si>
+    <t>OrchestratorTenancyName</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>The URL of your orchestrator server. This property is used only if you are using a Queue to store your Transaction Items.</t>
+  </si>
+  <si>
+    <t>The name of Orchestrator credentials. This should be stored in Windows Credential manager. This property is used only if you are using a Queue to store your Transaction Items.</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator tenant.  This property is used only if you are using a Queue to store your Transaction Items.</t>
   </si>
 </sst>
 </file>
@@ -568,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,53 +591,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -823,7 +813,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -834,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -845,7 +835,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -861,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes to wbLogging calls
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -36,166 +36,166 @@
     <t>Timeout short value in milliseconds, for activities which are likely to fail. Must be integer</t>
   </si>
   <si>
+    <t>TimeoutMedium</t>
+  </si>
+  <si>
+    <t>Timeout medium value in milliseconds. Must be integer</t>
+  </si>
+  <si>
+    <t>TimeoutLong</t>
+  </si>
+  <si>
+    <t>Timeout short value in milliseconds, for slow apps. Must be integer</t>
+  </si>
+  <si>
+    <t>ExScreenshotsFolderPath</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
+  </si>
+  <si>
+    <t>DelayShort</t>
+  </si>
+  <si>
+    <t>Delay short value in milliseconds, for activities where it is necessary to wait a little. Must be integer</t>
+  </si>
+  <si>
+    <t>DelayMedium</t>
+  </si>
+  <si>
+    <t>Delay medium value in milliseconds, for activities where it is necessary to wait a moderate amount of time. Must be integer</t>
+  </si>
+  <si>
+    <t>DelayLong</t>
+  </si>
+  <si>
+    <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
+  </si>
+  <si>
+    <t>AccuracyLow</t>
+  </si>
+  <si>
+    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
+  </si>
+  <si>
+    <t>AccuracyMedium</t>
+  </si>
+  <si>
+    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
+  </si>
+  <si>
+    <t>AccuracyHigh</t>
+  </si>
+  <si>
+    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data fetched succesfully for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_Success</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful</t>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException</t>
+  </si>
+  <si>
+    <t>Business rule exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception</t>
+  </si>
+  <si>
+    <t>LogMessage_ApplicationException</t>
+  </si>
+  <si>
+    <t>System exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception</t>
+  </si>
+  <si>
+    <t>OrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://demo.uipath.com</t>
+  </si>
+  <si>
+    <t>The URL of your orchestrator server. This property is used only if you are using a Queue to store your Transaction Items.</t>
+  </si>
+  <si>
+    <t>OrchestratorCredentialName</t>
+  </si>
+  <si>
+    <t>demo.uipath.com_credentials</t>
+  </si>
+  <si>
+    <t>The name of Orchestrator credentials. This should be stored in Windows Credential manager. This property is used only if you are using a Queue to store your Transaction Items.</t>
+  </si>
+  <si>
+    <t>OrchestratorTenancyName</t>
+  </si>
+  <si>
+    <t>fantastic</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator tenant.  This property is used only if you are using a Queue to store your Transaction Items.</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>KibanaDemoQueue</t>
+  </si>
+  <si>
+    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
+  </si>
+  <si>
+    <t>wbBusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>Task1</t>
+  </si>
+  <si>
+    <t>ServicesLayer\Task1\</t>
+  </si>
+  <si>
+    <t>The task name is used by the program to obtian the path to the slave program's root folder, relative to the main program's.</t>
+  </si>
+  <si>
     <t>Asset</t>
   </si>
   <si>
     <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>OrchestratorURL</t>
-  </si>
-  <si>
-    <t>https://demo.uipath.com</t>
-  </si>
-  <si>
-    <t>The URL of your orchestrator server. This property is used only if you are using a Queue to store your Transaction Items.</t>
-  </si>
-  <si>
-    <t>OrchestratorCredentialName</t>
-  </si>
-  <si>
-    <t>demo.uipath.com_credentials</t>
-  </si>
-  <si>
-    <t>The name of Orchestrator credentials. This should be stored in Windows Credential manager. This property is used only if you are using a Queue to store your Transaction Items.</t>
-  </si>
-  <si>
-    <t>OrchestratorTenancyName</t>
-  </si>
-  <si>
-    <t>fantastic</t>
-  </si>
-  <si>
-    <t>The name of the Orchestrator tenant.  This property is used only if you are using a Queue to store your Transaction Items.</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>KibanaDemoQueue</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
-  </si>
-  <si>
-    <t>wbBusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
-  </si>
-  <si>
-    <t>Task1</t>
-  </si>
-  <si>
-    <t>ServicesLayer\Task1\</t>
-  </si>
-  <si>
-    <t>The task name is used by the program to obtian the path to the slave program's root folder, relative to the main program's.</t>
-  </si>
-  <si>
-    <t>TimeoutMedium</t>
-  </si>
-  <si>
-    <t>Timeout medium value in milliseconds. Must be integer</t>
-  </si>
-  <si>
-    <t>TimeoutLong</t>
-  </si>
-  <si>
-    <t>Timeout short value in milliseconds, for slow apps. Must be integer</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
-  </si>
-  <si>
-    <t>DelayShort</t>
-  </si>
-  <si>
-    <t>Delay short value in milliseconds, for activities where it is necessary to wait a little. Must be integer</t>
-  </si>
-  <si>
-    <t>DelayMedium</t>
-  </si>
-  <si>
-    <t>Delay medium value in milliseconds, for activities where it is necessary to wait a moderate amount of time. Must be integer</t>
-  </si>
-  <si>
-    <t>DelayLong</t>
-  </si>
-  <si>
-    <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
-  </si>
-  <si>
-    <t>AccuracyLow</t>
-  </si>
-  <si>
-    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyMedium</t>
-  </si>
-  <si>
-    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyHigh</t>
-  </si>
-  <si>
-    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data fetched succesfully for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>System exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
 </sst>
 </file>
@@ -307,70 +307,70 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1"/>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1"/>
@@ -1421,8 +1421,8 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0.0</v>
+      <c r="B3" s="2">
+        <v>3.0</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1442,160 +1442,160 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>30000.0</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>120000.0</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1"/>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1000.0</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>15000.0</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>60000.0</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1"/>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1"/>
@@ -2594,10 +2594,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>

<commit_message>
Adding Suppress Successful Logging and wbTypes in Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11712" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Settings" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Constants" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Assets" sheetId="3" r:id="rId5"/>
+    <sheet name="Settings" sheetId="1" r:id="rId1"/>
+    <sheet name="Constants" sheetId="2" r:id="rId2"/>
+    <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -93,51 +101,6 @@
     <t>Image accuracy high value, for images that have low contrast. Must be double</t>
   </si>
   <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data fetched succesfully for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>System exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception</t>
-  </si>
-  <si>
     <t>OrchestratorURL</t>
   </si>
   <si>
@@ -196,82 +159,452 @@
   </si>
   <si>
     <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>wbInit_Type</t>
+  </si>
+  <si>
+    <t>MainTask, Initialization State</t>
+  </si>
+  <si>
+    <t>wbGetTransactionData_Type</t>
+  </si>
+  <si>
+    <t>MainTask, Get Transaction Data State</t>
+  </si>
+  <si>
+    <t>wbProcessTransaction_Type</t>
+  </si>
+  <si>
+    <t>MainTask, Process Transaction State</t>
+  </si>
+  <si>
+    <t>wbInit_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>wbGetTransactionData_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>wbProcessTransaction_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>Do not log successful executions of wb</t>
+  </si>
+  <si>
+    <t>wbCloseAllApplications_Type</t>
+  </si>
+  <si>
+    <t>wbCloseAllApplications_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>wbInitAllApplications_Type</t>
+  </si>
+  <si>
+    <t>wbInitAllApplications_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>wbProcess_Type</t>
+  </si>
+  <si>
+    <t>wbProcess_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>MainTask, Close All Applications</t>
+  </si>
+  <si>
+    <t>MainTask, InitAllApplications</t>
+  </si>
+  <si>
+    <t>MainTask, Process Transaction</t>
+  </si>
+  <si>
+    <t>Name of Workblock</t>
+  </si>
+  <si>
+    <t>MainTask, Next Transaction</t>
+  </si>
+  <si>
+    <t>wbNextTransaction_Type</t>
+  </si>
+  <si>
+    <t>wbNextTransaction_SuppressSuccessful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="68.0"/>
-    <col customWidth="1" min="2" max="2" width="70.14"/>
-    <col customWidth="1" min="3" max="3" width="68.57"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="68" customWidth="1"/>
+    <col min="2" max="2" width="70.109375" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -305,81 +638,81 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1365,24 +1698,27 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="53.0"/>
-    <col customWidth="1" min="2" max="2" width="63.57"/>
-    <col customWidth="1" min="3" max="3" width="89.0"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1416,54 +1752,54 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>30000.0</v>
+        <v>30000</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>120000.0</v>
+        <v>120000</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1474,42 +1810,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>15000.0</v>
+        <v>15000</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>60000.0</v>
+        <v>60000</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1520,7 +1856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1531,7 +1867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1542,71 +1878,161 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2574,30 +3000,33 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="65.43"/>
+    <col min="1" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2623,21 +3052,21 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3623,6 +4052,6 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wb Type changes in Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11712" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -164,21 +164,12 @@
     <t>wbInit_Type</t>
   </si>
   <si>
-    <t>MainTask, Initialization State</t>
-  </si>
-  <si>
     <t>wbGetTransactionData_Type</t>
   </si>
   <si>
-    <t>MainTask, Get Transaction Data State</t>
-  </si>
-  <si>
     <t>wbProcessTransaction_Type</t>
   </si>
   <si>
-    <t>MainTask, Process Transaction State</t>
-  </si>
-  <si>
     <t>wbInit_SuppressSuccessful</t>
   </si>
   <si>
@@ -209,25 +200,34 @@
     <t>wbProcess_SuppressSuccessful</t>
   </si>
   <si>
-    <t>MainTask, Close All Applications</t>
-  </si>
-  <si>
-    <t>MainTask, InitAllApplications</t>
-  </si>
-  <si>
-    <t>MainTask, Process Transaction</t>
-  </si>
-  <si>
     <t>Name of Workblock</t>
   </si>
   <si>
-    <t>MainTask, Next Transaction</t>
-  </si>
-  <si>
     <t>wbNextTransaction_Type</t>
   </si>
   <si>
     <t>wbNextTransaction_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>Main, FrameWork, Init</t>
+  </si>
+  <si>
+    <t>Main, Framework, GetData</t>
+  </si>
+  <si>
+    <t>Main, Framework, Process</t>
+  </si>
+  <si>
+    <t>Main, Framework, Next</t>
+  </si>
+  <si>
+    <t>Main, Business, CloseApps</t>
+  </si>
+  <si>
+    <t>Main, Business, InitApps</t>
+  </si>
+  <si>
+    <t>Main, Business, Process</t>
   </si>
 </sst>
 </file>
@@ -596,12 +596,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.109375" customWidth="1"/>
-    <col min="3" max="3" width="68.5546875" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1707,15 +1707,15 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B19" sqref="B19:B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="2" max="2" width="63.5703125" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1884,153 +1884,153 @@
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B26" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B28" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B30" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -3013,9 +3013,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added a new task, FirstRun. It can be scheduled to run once, when the program is in the Init stage, after the Config file has been read. It's data and operation are it's own. By default it does not run. You can change the behaviour from the main config.xlsx file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -146,15 +146,6 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>Task1</t>
-  </si>
-  <si>
-    <t>ServicesLayer\Task1\</t>
-  </si>
-  <si>
-    <t>The task name is used by the program to obtian the path to the slave program's root folder, relative to the main program's.</t>
-  </si>
-  <si>
     <t>Asset</t>
   </si>
   <si>
@@ -228,6 +219,70 @@
   </si>
   <si>
     <t>Main, Business, Process</t>
+  </si>
+  <si>
+    <t>FirstRun</t>
+  </si>
+  <si>
+    <t>ServicesLayer\FirstRun\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The task that executes first time programs starts. Responsible for its own configuration, data, processing, and retires. The task name value is used by the program to obtian the path to the slave program's root folder, relative to the main program's.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable the execution of the FirstRun Task. </t>
+  </si>
+  <si>
+    <t>wbFirstRunTask_Type</t>
+  </si>
+  <si>
+    <t>wbFirstRunTask_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>Main, Framework, FirstRun</t>
+  </si>
+  <si>
+    <t>Task1_FilePath</t>
+  </si>
+  <si>
+    <t>Task1_Name</t>
+  </si>
+  <si>
+    <t>Task1_Enable</t>
+  </si>
+  <si>
+    <t>Task name</t>
+  </si>
+  <si>
+    <t>Task path location</t>
+  </si>
+  <si>
+    <t>Enable Task setting.</t>
+  </si>
+  <si>
+    <t>Task2_Name</t>
+  </si>
+  <si>
+    <t>Task2_FilePath</t>
+  </si>
+  <si>
+    <t>Task2_Enable</t>
+  </si>
+  <si>
+    <t>Task3_Name</t>
+  </si>
+  <si>
+    <t>Task3_FilePath</t>
+  </si>
+  <si>
+    <t>Task3_Enable</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>ServicesLayer\unassigned\</t>
   </si>
 </sst>
 </file>
@@ -271,12 +326,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,15 +650,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
     <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -694,38 +754,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2"/>
+    </row>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1"/>
     <row r="32" ht="14.25" customHeight="1"/>
@@ -1697,6 +1728,8 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1704,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1881,174 +1914,283 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B22" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B24" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B26" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B28" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B30" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B32" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -3002,6 +3144,8 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3023,10 +3167,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>

<commit_message>
RunFrist task disabled by default. Enable in Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Main, Business, Process</t>
-  </si>
-  <si>
-    <t>FirstRun</t>
   </si>
   <si>
     <t>ServicesLayer\FirstRun\</t>
@@ -283,6 +280,21 @@
   </si>
   <si>
     <t>Task3_ServiceEnv</t>
+  </si>
+  <si>
+    <t>GetDataService</t>
+  </si>
+  <si>
+    <t>FirstRunService</t>
+  </si>
+  <si>
+    <t>wbGetDataTask_Type</t>
+  </si>
+  <si>
+    <t>wbGetDataTask_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>Main, Framework, GetData Service</t>
   </si>
 </sst>
 </file>
@@ -1737,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1936,10 +1948,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
         <v>56</v>
@@ -1947,7 +1959,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="3" t="b">
         <v>1</v>
@@ -1980,10 +1992,10 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
@@ -1991,7 +2003,7 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="B26" s="3" t="b">
         <v>1</v>
@@ -2002,10 +2014,10 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>62</v>
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
@@ -2013,7 +2025,7 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B28" s="3" t="b">
         <v>1</v>
@@ -2024,10 +2036,10 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>56</v>
@@ -2035,7 +2047,7 @@
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="b">
         <v>1</v>
@@ -2046,10 +2058,10 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
         <v>56</v>
@@ -2057,7 +2069,7 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" s="3" t="b">
         <v>1</v>
@@ -2068,10 +2080,10 @@
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
         <v>56</v>
@@ -2079,86 +2091,86 @@
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="2" t="s">
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1">
+      <c r="A38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
         <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -2167,28 +2179,48 @@
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
         <v>81</v>
       </c>
-      <c r="B44" t="b">
+      <c r="C44" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" t="b">
         <v>0</v>
       </c>
-      <c r="C44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="C46" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
@@ -3146,6 +3178,8 @@
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Two new tasks added, and the posibility to run a third. FirstRun service task is a componetn run once, at program start. GetData is a service component whose run frequency can be configured from the invoker's (Main framework) config. It can be disabled, run once, or run for every transaction. It enables fetching of remote data, where exceptions are the norm. It returns TransactionData
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -231,70 +231,55 @@
     <t xml:space="preserve">Enable the execution of the FirstRun Task. </t>
   </si>
   <si>
-    <t>wbFirstRunTask_Type</t>
-  </si>
-  <si>
-    <t>wbFirstRunTask_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>Main, Framework, FirstRun</t>
-  </si>
-  <si>
-    <t>Task1_Name</t>
-  </si>
-  <si>
-    <t>Task1_Enable</t>
-  </si>
-  <si>
     <t>Task name</t>
   </si>
   <si>
     <t>Task path location</t>
   </si>
   <si>
-    <t>Enable Task setting.</t>
-  </si>
-  <si>
-    <t>Task2_Name</t>
-  </si>
-  <si>
-    <t>Task2_Enable</t>
-  </si>
-  <si>
-    <t>Task3_Name</t>
-  </si>
-  <si>
-    <t>Task3_Enable</t>
-  </si>
-  <si>
-    <t>unassigned</t>
-  </si>
-  <si>
-    <t>ServicesLayer\unassigned\</t>
-  </si>
-  <si>
-    <t>Task2_ServiceEnv</t>
-  </si>
-  <si>
-    <t>Task1_ServiceEnv</t>
-  </si>
-  <si>
-    <t>Task3_ServiceEnv</t>
-  </si>
-  <si>
-    <t>GetDataService</t>
-  </si>
-  <si>
-    <t>FirstRunService</t>
-  </si>
-  <si>
-    <t>wbGetDataTask_Type</t>
-  </si>
-  <si>
-    <t>wbGetDataTask_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>Main, Framework, GetData Service</t>
+    <t>Key is the TaskName and value is the Task Environment (path)</t>
+  </si>
+  <si>
+    <t>SystemTask1_Name</t>
+  </si>
+  <si>
+    <t>SystemTask1_Env</t>
+  </si>
+  <si>
+    <t>SystemTask1_Enable</t>
+  </si>
+  <si>
+    <t>SystemTask2_Name</t>
+  </si>
+  <si>
+    <t>SystemTask2_Env</t>
+  </si>
+  <si>
+    <t>SystemTask2_Enable</t>
+  </si>
+  <si>
+    <t>Main, Framework, FirstRun Task</t>
+  </si>
+  <si>
+    <t>Main, Framework, GetData Task</t>
+  </si>
+  <si>
+    <t>ServicesLayer\GetData\</t>
+  </si>
+  <si>
+    <t>Enable Task setting. [0=Disable. 1=Enable during first run, 2=Always enable]</t>
+  </si>
+  <si>
+    <t>Task1</t>
+  </si>
+  <si>
+    <t>ServicesLayer\Task1</t>
+  </si>
+  <si>
+    <t>Task2</t>
+  </si>
+  <si>
+    <t>ServicesLayer\Task2</t>
   </si>
 </sst>
 </file>
@@ -338,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -347,6 +332,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,7 +656,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -768,6 +759,28 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1"/>
@@ -1749,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1948,10 +1961,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
         <v>56</v>
@@ -1959,7 +1972,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="b">
         <v>1</v>
@@ -1970,10 +1983,10 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
         <v>56</v>
@@ -1981,7 +1994,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="3" t="b">
         <v>1</v>
@@ -1992,10 +2005,10 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
@@ -2003,7 +2016,7 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B26" s="3" t="b">
         <v>1</v>
@@ -2014,10 +2027,10 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
+        <v>50</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
@@ -2025,7 +2038,7 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B28" s="3" t="b">
         <v>1</v>
@@ -2036,10 +2049,10 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>62</v>
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>56</v>
@@ -2047,7 +2060,7 @@
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B30" s="3" t="b">
         <v>1</v>
@@ -2058,10 +2071,10 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
         <v>56</v>
@@ -2069,158 +2082,89 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B32" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" t="s">
-        <v>56</v>
-      </c>
-    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="3" t="b">
+        <v>72</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="b">
         <v>1</v>
       </c>
-      <c r="C34" t="s">
-        <v>49</v>
+      <c r="C36" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>56</v>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1">
-      <c r="A38" s="2" t="s">
-        <v>72</v>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" t="b">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46" t="s">
-        <v>76</v>
-      </c>
-    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
@@ -3173,13 +3117,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
-    <row r="1004" ht="14.25" customHeight="1"/>
-    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed default service options
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2119,7 +2119,7 @@
         <v>74</v>
       </c>
       <c r="B36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Added Retry for Init State. Configurable through Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
   </si>
   <si>
     <t>TimeoutShort</t>
@@ -280,6 +277,15 @@
   </si>
   <si>
     <t>ServicesLayer\Task2</t>
+  </si>
+  <si>
+    <t>MaxInitRetryNumber</t>
+  </si>
+  <si>
+    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
+  </si>
+  <si>
+    <t>If &gt; 0 will retry the Initialisation state with a failed exception.</t>
   </si>
 </sst>
 </file>
@@ -703,58 +709,58 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -762,24 +768,24 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
@@ -1764,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -1819,343 +1825,353 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>5000</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>30000</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>120000</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1000</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>15000</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>60000</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B36" t="b">
         <v>0</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" s="6">
         <v>0</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3138,10 +3154,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>

<commit_message>
added workblocks sheet to config files and tasks sheet only to main config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -13,15 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Constants" sheetId="2" r:id="rId2"/>
-    <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="Workblocks" sheetId="4" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="5" r:id="rId3"/>
+    <sheet name="Constants" sheetId="2" r:id="rId4"/>
+    <sheet name="Assets" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -329,18 +331,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -662,7 +658,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -765,28 +761,6 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="A9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1"/>
@@ -1767,11 +1741,315 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z998"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z999"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1839,350 +2117,148 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>5000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>30000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>120000</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>1000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>15000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>60000</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>0.6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>0.9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1">
-      <c r="A35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="6">
-        <v>0</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -3133,12 +3209,13 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>

</xml_diff>

<commit_message>
Default config setting change
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1744,7 +1744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1929,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
First run now uses a List(of Tuple(of x, y)) as TransactionData and a Tuple as TransactionItem.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -288,6 +288,21 @@
   </si>
   <si>
     <t>If &gt; 0 will retry the Initialisation state with a failed exception.</t>
+  </si>
+  <si>
+    <t>Debug_wbSaveReport</t>
+  </si>
+  <si>
+    <t>Debug_wbSaveReportPath</t>
+  </si>
+  <si>
+    <t>Set to TRUE to enable storage of each application run. It contains a detailed report, per Workblock executed</t>
+  </si>
+  <si>
+    <t>Path to save the reports. Relative or absolute</t>
+  </si>
+  <si>
+    <t>Data\Output\</t>
   </si>
 </sst>
 </file>
@@ -657,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -761,6 +776,28 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1"/>
@@ -1929,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
TransactionItem can now also be written in the Process Layer. It is thus i/o. This reflects a duality of processes, some of which have data readily available and need only process it, others whose purpose is just to obtain data for later processing.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1966,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2015,7 +2015,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Added wbKey wbPath to wbLogging and updated the interface across the project
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -197,27 +197,6 @@
   </si>
   <si>
     <t>wbNextTransaction_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>Main, FrameWork, Init</t>
-  </si>
-  <si>
-    <t>Main, Framework, GetData</t>
-  </si>
-  <si>
-    <t>Main, Framework, Process</t>
-  </si>
-  <si>
-    <t>Main, Framework, Next</t>
-  </si>
-  <si>
-    <t>Main, Business, CloseApps</t>
-  </si>
-  <si>
-    <t>Main, Business, InitApps</t>
-  </si>
-  <si>
-    <t>Main, Business, Process</t>
   </si>
   <si>
     <t>ServicesLayer\FirstRun\</t>
@@ -257,12 +236,6 @@
     <t>SystemTask2_Enable</t>
   </si>
   <si>
-    <t>Main, Framework, FirstRun Task</t>
-  </si>
-  <si>
-    <t>Main, Framework, GetData Task</t>
-  </si>
-  <si>
     <t>ServicesLayer\GetData\</t>
   </si>
   <si>
@@ -303,6 +276,42 @@
   </si>
   <si>
     <t>Data\Output\</t>
+  </si>
+  <si>
+    <t>wbCloseAppsRecover_Type</t>
+  </si>
+  <si>
+    <t>wbCloseAppsRecover_SuppressSuccessful</t>
+  </si>
+  <si>
+    <t>Init</t>
+  </si>
+  <si>
+    <t>GetData</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>CloseApps</t>
+  </si>
+  <si>
+    <t>InitApps</t>
+  </si>
+  <si>
+    <t>RecoverApps</t>
+  </si>
+  <si>
+    <t>ProcessApps</t>
+  </si>
+  <si>
+    <t>FirstRunTask</t>
+  </si>
+  <si>
+    <t>GetDataTask</t>
   </si>
 </sst>
 </file>
@@ -779,24 +788,24 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
@@ -1779,7 +1788,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -1788,7 +1797,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1808,7 +1817,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>55</v>
@@ -1827,10 +1836,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -1838,7 +1847,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -1849,10 +1858,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>55</v>
@@ -1860,7 +1869,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>1</v>
@@ -1871,10 +1880,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>55</v>
@@ -1882,7 +1891,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="b">
         <v>1</v>
@@ -1893,10 +1902,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>55</v>
@@ -1904,7 +1913,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3" t="b">
         <v>1</v>
@@ -1915,10 +1924,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
+        <v>49</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
@@ -1926,7 +1935,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="b">
         <v>1</v>
@@ -1937,10 +1946,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
         <v>55</v>
@@ -1948,12 +1957,34 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="3" t="b">
+      <c r="B18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1967,7 +1998,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1990,90 +2021,90 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2140,18 +2171,18 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
BusinessRuleException is no longer caught in a seperate catch, but it is identifeid as such in the System.Exception general catch using the exception.GetType.Name property
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -311,7 +311,7 @@
     <t>GetDataTask</t>
   </si>
   <si>
-    <t>KibanaQueue_ArchConnect</t>
+    <t>REFrameWork</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -791,7 +791,7 @@
         <v>78</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>80</v>
@@ -1998,7 +1998,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2046,7 +2046,7 @@
         <v>65</v>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
NextTransaction.xaml deleted and replaced with actions in transitions.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -188,12 +188,6 @@
   </si>
   <si>
     <t>Name of Workblock</t>
-  </si>
-  <si>
-    <t>wbNextTransaction_Type</t>
-  </si>
-  <si>
-    <t>wbNextTransaction_SuppressSuccessful</t>
   </si>
   <si>
     <t>ServicesLayer\FirstRun\</t>
@@ -288,9 +282,6 @@
   </si>
   <si>
     <t>Process</t>
-  </si>
-  <si>
-    <t>Next</t>
   </si>
   <si>
     <t>CloseApps</t>
@@ -681,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -777,7 +768,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -788,24 +779,24 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
@@ -1788,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1817,7 +1808,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -1836,10 +1827,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
@@ -1847,7 +1838,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -1861,7 +1852,7 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -1883,7 +1874,7 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -1902,10 +1893,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
+        <v>48</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -1913,7 +1904,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="b">
         <v>1</v>
@@ -1924,10 +1915,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>89</v>
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
@@ -1935,7 +1926,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B14" s="3" t="b">
         <v>1</v>
@@ -1946,10 +1937,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
@@ -1957,34 +1948,12 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1997,7 +1966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2021,90 +1990,90 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>67</v>
       </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2171,18 +2140,18 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added MaxContinuousRetryNumber as a method for the process to fail if we have many consecutive fails at the Process State. After all, you sometimes do not want to consume your TransactionItems when the application portal is offline, and would rather fail after receiving many consecutive Application Exceptions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -248,12 +248,6 @@
     <t>MaxInitRetryNumber</t>
   </si>
   <si>
-    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
-  </si>
-  <si>
-    <t>If &gt; 0 will retry the Initialisation state with a failed exception.</t>
-  </si>
-  <si>
     <t>Debug_wbSaveReport</t>
   </si>
   <si>
@@ -303,6 +297,18 @@
   </si>
   <si>
     <t>REFrameWork</t>
+  </si>
+  <si>
+    <t>MaxContinuousRetryNumber</t>
+  </si>
+  <si>
+    <t>If &gt; 0 will retry the Initialisation state with a failed exception. Must be an integer.</t>
+  </si>
+  <si>
+    <t>If &gt; 0 will keep a record of consecutive failed exceptions of the Process state. When this number is reached, the application will fail. Must be an integer.</t>
+  </si>
+  <si>
+    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -779,24 +785,24 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
@@ -1808,7 +1814,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -1827,10 +1833,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
@@ -1838,7 +1844,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -1852,7 +1858,7 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -1874,7 +1880,7 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -1896,7 +1902,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -1918,7 +1924,7 @@
         <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
@@ -1940,7 +1946,7 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
@@ -1993,7 +1999,7 @@
         <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -2026,7 +2032,7 @@
         <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>58</v>
@@ -2083,10 +2089,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2140,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2151,124 +2157,134 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>5000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>30000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>120000</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>1000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>15000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>60000</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>0.6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0.8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>0.9</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2285,7 +2301,7 @@
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
     <row r="39" ht="14.25" customHeight="1"/>
     <row r="40" ht="14.25" customHeight="1"/>
     <row r="41" ht="14.25" customHeight="1"/>
@@ -3247,6 +3263,7 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed default MaxContinuousRetryNumber to 9 instead of 0
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1972,7 +1972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2091,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2165,7 +2165,7 @@
         <v>91</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
CloseAllApplications.xaml and InitAllApplications.xaml no longer contain a workblock by default, both at main level as well as service levels. In addition, workflows that contain workblock no longer pass in_wbType, as the same of the workblock is to be decided inside the workflow (a workflow can contain multiple workblocks).
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -167,24 +167,6 @@
   </si>
   <si>
     <t>Do not log successful executions of wb</t>
-  </si>
-  <si>
-    <t>wbCloseAllApplications_Type</t>
-  </si>
-  <si>
-    <t>wbCloseAllApplications_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>wbInitAllApplications_Type</t>
-  </si>
-  <si>
-    <t>wbInitAllApplications_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>wbProcess_Type</t>
-  </si>
-  <si>
-    <t>wbProcess_SuppressSuccessful</t>
   </si>
   <si>
     <t>Name of Workblock</t>
@@ -200,27 +182,18 @@
     <t xml:space="preserve">Enable the execution of the FirstRun Task. </t>
   </si>
   <si>
-    <t>Task name</t>
-  </si>
-  <si>
     <t>Task path location</t>
   </si>
   <si>
     <t>Key is the TaskName and value is the Task Environment (path)</t>
   </si>
   <si>
-    <t>SystemTask1_Name</t>
-  </si>
-  <si>
     <t>SystemTask1_Env</t>
   </si>
   <si>
     <t>SystemTask1_Enable</t>
   </si>
   <si>
-    <t>SystemTask2_Name</t>
-  </si>
-  <si>
     <t>SystemTask2_Env</t>
   </si>
   <si>
@@ -263,12 +236,6 @@
     <t>Data\Output\</t>
   </si>
   <si>
-    <t>wbCloseAppsRecover_Type</t>
-  </si>
-  <si>
-    <t>wbCloseAppsRecover_SuppressSuccessful</t>
-  </si>
-  <si>
     <t>Init</t>
   </si>
   <si>
@@ -276,24 +243,6 @@
   </si>
   <si>
     <t>Process</t>
-  </si>
-  <si>
-    <t>CloseApps</t>
-  </si>
-  <si>
-    <t>InitApps</t>
-  </si>
-  <si>
-    <t>RecoverApps</t>
-  </si>
-  <si>
-    <t>ProcessApps</t>
-  </si>
-  <si>
-    <t>FirstRunTask</t>
-  </si>
-  <si>
-    <t>GetDataTask</t>
   </si>
   <si>
     <t>REFrameWork</t>
@@ -774,7 +723,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -785,24 +734,24 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
@@ -1785,10 +1734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A3" sqref="A3:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1814,10 +1763,10 @@
         <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1833,18 +1782,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -1855,111 +1804,23 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1970,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1996,90 +1857,68 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C4" t="s">
-        <v>56</v>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>57</v>
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>89</v>
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>68</v>
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +1930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2146,29 +1985,29 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Run reports can now be output in json or csv format (setting in COnfix.xlsx). Tests now output csv format
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806497E8-4747-4073-8469-8AF422443052}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -258,6 +259,15 @@
   </si>
   <si>
     <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
+  </si>
+  <si>
+    <t>Debug_wbFileFormat</t>
+  </si>
+  <si>
+    <t>Options are csv and json. Default option is csv</t>
+  </si>
+  <si>
+    <t>csv</t>
   </si>
 </sst>
 </file>
@@ -627,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -752,6 +762,17 @@
       </c>
       <c r="C10" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
@@ -1736,7 +1757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1834,7 +1855,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1893,7 +1914,7 @@
         <v>57</v>
       </c>
       <c r="B6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Cleaned up ReFramework. It now default to an empty template.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806497E8-4747-4073-8469-8AF422443052}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6374A9FB-01BE-4D43-A4D5-85DD15FC669C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -104,34 +104,22 @@
     <t>OrchestratorURL</t>
   </si>
   <si>
-    <t>https://demo.uipath.com</t>
-  </si>
-  <si>
     <t>The URL of your orchestrator server. This property is used only if you are using a Queue to store your Transaction Items.</t>
   </si>
   <si>
     <t>OrchestratorCredentialName</t>
   </si>
   <si>
-    <t>demo.uipath.com_credentials</t>
-  </si>
-  <si>
     <t>The name of Orchestrator credentials. This should be stored in Windows Credential manager. This property is used only if you are using a Queue to store your Transaction Items.</t>
   </si>
   <si>
     <t>OrchestratorTenancyName</t>
   </si>
   <si>
-    <t>fantastic</t>
-  </si>
-  <si>
     <t>The name of the Orchestrator tenant.  This property is used only if you are using a Queue to store your Transaction Items.</t>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>KibanaDemoQueue</t>
   </si>
   <si>
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
@@ -637,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -687,56 +675,44 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -744,36 +720,42 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
-      </c>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1">
+      <c r="B14" s="4"/>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1"/>
@@ -1781,68 +1763,68 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1854,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1878,68 +1860,68 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2006,29 +1988,29 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3145,10 +3127,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>

<commit_message>
Minor adjustments in code. Introduction page to Config.xlsx, to be filled with instructions for dictionary usage. Keys marked according to usage
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6374A9FB-01BE-4D43-A4D5-85DD15FC669C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A624D-75A4-4BDE-A3FA-F3F0BEDE8D9A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Workblocks" sheetId="4" r:id="rId2"/>
-    <sheet name="Tasks" sheetId="5" r:id="rId3"/>
-    <sheet name="Constants" sheetId="2" r:id="rId4"/>
-    <sheet name="Assets" sheetId="3" r:id="rId5"/>
+    <sheet name="Introduction" sheetId="7" r:id="rId1"/>
+    <sheet name="Settings" sheetId="1" r:id="rId2"/>
+    <sheet name="Credentials" sheetId="6" r:id="rId3"/>
+    <sheet name="Workblocks" sheetId="4" r:id="rId4"/>
+    <sheet name="Tasks" sheetId="5" r:id="rId5"/>
+    <sheet name="Constants" sheetId="2" r:id="rId6"/>
+    <sheet name="Assets" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -256,13 +258,34 @@
   </si>
   <si>
     <t>csv</t>
+  </si>
+  <si>
+    <t>####  Legend ####</t>
+  </si>
+  <si>
+    <t>Help. To be written</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
+  </si>
+  <si>
+    <t>This Key is used only during Debug. You can delete in production</t>
+  </si>
+  <si>
+    <t>This key belongs to user designated category 1</t>
+  </si>
+  <si>
+    <t>This key is used in the Framework layer. You can change the values, but do not delete the keys</t>
+  </si>
+  <si>
+    <t>This key is used in the Business Process Layer. The developer is responsible for the keys. The user is responsible for the values.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -278,16 +301,68 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -295,11 +370,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -309,9 +418,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,11 +742,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="45">
+      <c r="A10" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -672,91 +845,66 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>25</v>
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>27</v>
+    <row r="3" spans="1:26" ht="15" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>29</v>
+    <row r="4" spans="1:26" ht="15" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
+    <row r="5" spans="1:26" ht="15" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
+    <row r="8" spans="1:26" ht="15" customHeight="1">
+      <c r="B8" s="4"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1">
-      <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1">
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="B14" s="4"/>
-    </row>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1"/>
     <row r="32" ht="14.25" customHeight="1"/>
@@ -1724,224 +1872,25 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC672C-F735-4EF3-8287-9B35E6A7A36A}">
+  <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="89" customWidth="1"/>
+    <col min="1" max="1" width="68" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1979,43 +1928,1299 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3</v>
+      <c r="A3" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
+    <row r="798" ht="14.25" customHeight="1"/>
+    <row r="799" ht="14.25" customHeight="1"/>
+    <row r="800" ht="14.25" customHeight="1"/>
+    <row r="801" ht="14.25" customHeight="1"/>
+    <row r="802" ht="14.25" customHeight="1"/>
+    <row r="803" ht="14.25" customHeight="1"/>
+    <row r="804" ht="14.25" customHeight="1"/>
+    <row r="805" ht="14.25" customHeight="1"/>
+    <row r="806" ht="14.25" customHeight="1"/>
+    <row r="807" ht="14.25" customHeight="1"/>
+    <row r="808" ht="14.25" customHeight="1"/>
+    <row r="809" ht="14.25" customHeight="1"/>
+    <row r="810" ht="14.25" customHeight="1"/>
+    <row r="811" ht="14.25" customHeight="1"/>
+    <row r="812" ht="14.25" customHeight="1"/>
+    <row r="813" ht="14.25" customHeight="1"/>
+    <row r="814" ht="14.25" customHeight="1"/>
+    <row r="815" ht="14.25" customHeight="1"/>
+    <row r="816" ht="14.25" customHeight="1"/>
+    <row r="817" ht="14.25" customHeight="1"/>
+    <row r="818" ht="14.25" customHeight="1"/>
+    <row r="819" ht="14.25" customHeight="1"/>
+    <row r="820" ht="14.25" customHeight="1"/>
+    <row r="821" ht="14.25" customHeight="1"/>
+    <row r="822" ht="14.25" customHeight="1"/>
+    <row r="823" ht="14.25" customHeight="1"/>
+    <row r="824" ht="14.25" customHeight="1"/>
+    <row r="825" ht="14.25" customHeight="1"/>
+    <row r="826" ht="14.25" customHeight="1"/>
+    <row r="827" ht="14.25" customHeight="1"/>
+    <row r="828" ht="14.25" customHeight="1"/>
+    <row r="829" ht="14.25" customHeight="1"/>
+    <row r="830" ht="14.25" customHeight="1"/>
+    <row r="831" ht="14.25" customHeight="1"/>
+    <row r="832" ht="14.25" customHeight="1"/>
+    <row r="833" ht="14.25" customHeight="1"/>
+    <row r="834" ht="14.25" customHeight="1"/>
+    <row r="835" ht="14.25" customHeight="1"/>
+    <row r="836" ht="14.25" customHeight="1"/>
+    <row r="837" ht="14.25" customHeight="1"/>
+    <row r="838" ht="14.25" customHeight="1"/>
+    <row r="839" ht="14.25" customHeight="1"/>
+    <row r="840" ht="14.25" customHeight="1"/>
+    <row r="841" ht="14.25" customHeight="1"/>
+    <row r="842" ht="14.25" customHeight="1"/>
+    <row r="843" ht="14.25" customHeight="1"/>
+    <row r="844" ht="14.25" customHeight="1"/>
+    <row r="845" ht="14.25" customHeight="1"/>
+    <row r="846" ht="14.25" customHeight="1"/>
+    <row r="847" ht="14.25" customHeight="1"/>
+    <row r="848" ht="14.25" customHeight="1"/>
+    <row r="849" ht="14.25" customHeight="1"/>
+    <row r="850" ht="14.25" customHeight="1"/>
+    <row r="851" ht="14.25" customHeight="1"/>
+    <row r="852" ht="14.25" customHeight="1"/>
+    <row r="853" ht="14.25" customHeight="1"/>
+    <row r="854" ht="14.25" customHeight="1"/>
+    <row r="855" ht="14.25" customHeight="1"/>
+    <row r="856" ht="14.25" customHeight="1"/>
+    <row r="857" ht="14.25" customHeight="1"/>
+    <row r="858" ht="14.25" customHeight="1"/>
+    <row r="859" ht="14.25" customHeight="1"/>
+    <row r="860" ht="14.25" customHeight="1"/>
+    <row r="861" ht="14.25" customHeight="1"/>
+    <row r="862" ht="14.25" customHeight="1"/>
+    <row r="863" ht="14.25" customHeight="1"/>
+    <row r="864" ht="14.25" customHeight="1"/>
+    <row r="865" ht="14.25" customHeight="1"/>
+    <row r="866" ht="14.25" customHeight="1"/>
+    <row r="867" ht="14.25" customHeight="1"/>
+    <row r="868" ht="14.25" customHeight="1"/>
+    <row r="869" ht="14.25" customHeight="1"/>
+    <row r="870" ht="14.25" customHeight="1"/>
+    <row r="871" ht="14.25" customHeight="1"/>
+    <row r="872" ht="14.25" customHeight="1"/>
+    <row r="873" ht="14.25" customHeight="1"/>
+    <row r="874" ht="14.25" customHeight="1"/>
+    <row r="875" ht="14.25" customHeight="1"/>
+    <row r="876" ht="14.25" customHeight="1"/>
+    <row r="877" ht="14.25" customHeight="1"/>
+    <row r="878" ht="14.25" customHeight="1"/>
+    <row r="879" ht="14.25" customHeight="1"/>
+    <row r="880" ht="14.25" customHeight="1"/>
+    <row r="881" ht="14.25" customHeight="1"/>
+    <row r="882" ht="14.25" customHeight="1"/>
+    <row r="883" ht="14.25" customHeight="1"/>
+    <row r="884" ht="14.25" customHeight="1"/>
+    <row r="885" ht="14.25" customHeight="1"/>
+    <row r="886" ht="14.25" customHeight="1"/>
+    <row r="887" ht="14.25" customHeight="1"/>
+    <row r="888" ht="14.25" customHeight="1"/>
+    <row r="889" ht="14.25" customHeight="1"/>
+    <row r="890" ht="14.25" customHeight="1"/>
+    <row r="891" ht="14.25" customHeight="1"/>
+    <row r="892" ht="14.25" customHeight="1"/>
+    <row r="893" ht="14.25" customHeight="1"/>
+    <row r="894" ht="14.25" customHeight="1"/>
+    <row r="895" ht="14.25" customHeight="1"/>
+    <row r="896" ht="14.25" customHeight="1"/>
+    <row r="897" ht="14.25" customHeight="1"/>
+    <row r="898" ht="14.25" customHeight="1"/>
+    <row r="899" ht="14.25" customHeight="1"/>
+    <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25" customHeight="1"/>
+    <row r="903" ht="14.25" customHeight="1"/>
+    <row r="904" ht="14.25" customHeight="1"/>
+    <row r="905" ht="14.25" customHeight="1"/>
+    <row r="906" ht="14.25" customHeight="1"/>
+    <row r="907" ht="14.25" customHeight="1"/>
+    <row r="908" ht="14.25" customHeight="1"/>
+    <row r="909" ht="14.25" customHeight="1"/>
+    <row r="910" ht="14.25" customHeight="1"/>
+    <row r="911" ht="14.25" customHeight="1"/>
+    <row r="912" ht="14.25" customHeight="1"/>
+    <row r="913" ht="14.25" customHeight="1"/>
+    <row r="914" ht="14.25" customHeight="1"/>
+    <row r="915" ht="14.25" customHeight="1"/>
+    <row r="916" ht="14.25" customHeight="1"/>
+    <row r="917" ht="14.25" customHeight="1"/>
+    <row r="918" ht="14.25" customHeight="1"/>
+    <row r="919" ht="14.25" customHeight="1"/>
+    <row r="920" ht="14.25" customHeight="1"/>
+    <row r="921" ht="14.25" customHeight="1"/>
+    <row r="922" ht="14.25" customHeight="1"/>
+    <row r="923" ht="14.25" customHeight="1"/>
+    <row r="924" ht="14.25" customHeight="1"/>
+    <row r="925" ht="14.25" customHeight="1"/>
+    <row r="926" ht="14.25" customHeight="1"/>
+    <row r="927" ht="14.25" customHeight="1"/>
+    <row r="928" ht="14.25" customHeight="1"/>
+    <row r="929" ht="14.25" customHeight="1"/>
+    <row r="930" ht="14.25" customHeight="1"/>
+    <row r="931" ht="14.25" customHeight="1"/>
+    <row r="932" ht="14.25" customHeight="1"/>
+    <row r="933" ht="14.25" customHeight="1"/>
+    <row r="934" ht="14.25" customHeight="1"/>
+    <row r="935" ht="14.25" customHeight="1"/>
+    <row r="936" ht="14.25" customHeight="1"/>
+    <row r="937" ht="14.25" customHeight="1"/>
+    <row r="938" ht="14.25" customHeight="1"/>
+    <row r="939" ht="14.25" customHeight="1"/>
+    <row r="940" ht="14.25" customHeight="1"/>
+    <row r="941" ht="14.25" customHeight="1"/>
+    <row r="942" ht="14.25" customHeight="1"/>
+    <row r="943" ht="14.25" customHeight="1"/>
+    <row r="944" ht="14.25" customHeight="1"/>
+    <row r="945" ht="14.25" customHeight="1"/>
+    <row r="946" ht="14.25" customHeight="1"/>
+    <row r="947" ht="14.25" customHeight="1"/>
+    <row r="948" ht="14.25" customHeight="1"/>
+    <row r="949" ht="14.25" customHeight="1"/>
+    <row r="950" ht="14.25" customHeight="1"/>
+    <row r="951" ht="14.25" customHeight="1"/>
+    <row r="952" ht="14.25" customHeight="1"/>
+    <row r="953" ht="14.25" customHeight="1"/>
+    <row r="954" ht="14.25" customHeight="1"/>
+    <row r="955" ht="14.25" customHeight="1"/>
+    <row r="956" ht="14.25" customHeight="1"/>
+    <row r="957" ht="14.25" customHeight="1"/>
+    <row r="958" ht="14.25" customHeight="1"/>
+    <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
+    <row r="962" ht="14.25" customHeight="1"/>
+    <row r="963" ht="14.25" customHeight="1"/>
+    <row r="964" ht="14.25" customHeight="1"/>
+    <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
+    <row r="975" ht="14.25" customHeight="1"/>
+    <row r="976" ht="14.25" customHeight="1"/>
+    <row r="977" ht="14.25" customHeight="1"/>
+    <row r="978" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
+    <row r="982" ht="14.25" customHeight="1"/>
+    <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
+    <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z998"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="B4">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B7">
@@ -2026,7 +3231,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -2037,7 +3242,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -2049,84 +3254,74 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1000</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>15000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>13</v>
+      <c r="A13" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>15000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>60000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>0.8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>19</v>
+      <c r="A17" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B17">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>0.8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <v>0.9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2142,8 +3337,8 @@
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
     <row r="39" ht="14.25" customHeight="1"/>
     <row r="40" ht="14.25" customHeight="1"/>
     <row r="41" ht="14.25" customHeight="1"/>
@@ -3104,14 +4299,12 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>

</xml_diff>

<commit_message>
Formatted introduction sheet from Config.xlsx
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A624D-75A4-4BDE-A3FA-F3F0BEDE8D9A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB8D664-6B01-467F-AF41-158D9C021C81}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,12 +260,6 @@
     <t>csv</t>
   </si>
   <si>
-    <t>####  Legend ####</t>
-  </si>
-  <si>
-    <t>Help. To be written</t>
-  </si>
-  <si>
     <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
   </si>
   <si>
@@ -279,13 +273,19 @@
   </si>
   <si>
     <t>This key is used in the Business Process Layer. The developer is responsible for the keys. The user is responsible for the values.</t>
+  </si>
+  <si>
+    <t>Help regarding this Configuration File</t>
+  </si>
+  <si>
+    <t>####  Legend of Key Value pairs####</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -328,6 +328,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -408,7 +422,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -418,13 +432,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -743,54 +773,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="116.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="18.75">
+      <c r="A1" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30">
+      <c r="A4" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="13" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="45">
-      <c r="A10" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -845,7 +879,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
@@ -856,7 +890,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="b">
@@ -867,7 +901,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B4" t="s">
@@ -878,7 +912,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B5" t="s">
@@ -889,7 +923,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
@@ -1929,7 +1963,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
@@ -1937,7 +1971,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
@@ -1945,7 +1979,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
@@ -2935,7 +2969,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2957,7 +2991,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2968,7 +3002,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="3" t="b">
@@ -2979,7 +3013,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
@@ -2990,7 +3024,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="3" t="b">
@@ -3001,7 +3035,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B6" t="s">
@@ -3012,7 +3046,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="3" t="b">
@@ -3054,7 +3088,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B2" t="s">
@@ -3065,7 +3099,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B3" t="b">
@@ -3076,7 +3110,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B4" t="s">
@@ -3087,7 +3121,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="4">
@@ -3098,7 +3132,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B7" t="s">
@@ -3109,7 +3143,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B8" t="s">
@@ -3175,7 +3209,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
@@ -3186,7 +3220,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B3">
@@ -3197,7 +3231,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B4">
@@ -3208,7 +3242,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -3220,7 +3254,7 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B7">
@@ -3231,7 +3265,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -3242,7 +3276,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -3254,7 +3288,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B11">
@@ -3265,7 +3299,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B12">
@@ -3276,7 +3310,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13">
@@ -3288,7 +3322,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B15">
@@ -3299,7 +3333,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B16">
@@ -3310,7 +3344,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B17">

</xml_diff>

<commit_message>
Added Introduction and help in Config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB8D664-6B01-467F-AF41-158D9C021C81}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043FFA49-94A4-4929-93EF-C72B6878557D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -278,14 +278,62 @@
     <t>Help regarding this Configuration File</t>
   </si>
   <si>
-    <t>####  Legend of Key Value pairs####</t>
+    <t>This is the configuration file used to describe various changeable parameters of the process. You should use this file to store settings that are environment related (like paths to programs or resources), user related (email account names, credential names), or plain data (URL of website or name of SAP report to execute). Below, the purpose of each sheet is explained in more detail.</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Credentials</t>
+  </si>
+  <si>
+    <t>Workblocks</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>The credentials sheet is the place to store your credential names.There is also one special credential, that needs to be defined only once, and which is comprised of the URL, TenancyName and CredentialName required to authenticate to the Orchestrator server using REST API. This is only used when working with QueueItems.</t>
+  </si>
+  <si>
+    <t>The workblock names are of the states in the framework. Define the names of workblocks you create here.</t>
+  </si>
+  <si>
+    <t>FirstRunTask: This task is invoked in the Framework Layer and executes only once(Even if Transaction number 1 were to fail and be retried, it would not be executed again), at program startup. It should not interact with data in memory, since it executes before we enter the main process data layer, but it can be used as a queue dispatcher.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task1: This task is not invoked anywhere, and should be used by the developer. </t>
+  </si>
+  <si>
+    <t>The sheet contains the list of tasks. Each task is another Business Process Layer context that is executed at some point during the main process execution. For system tasks, the execution is preselected and configurable from the settings. For user added tasks, it is chosen by the user.</t>
+  </si>
+  <si>
+    <t>GetDataTask: This task is invoked in the Data Layer of the main task. The reason is that we might desire it to deliver some TransactionData to us is a safe manner. Thus, it might navigate a website, download a file, process it, and deliver us an output datatable TransactionData. This would be made available in the Data Layer of the main task and would be ready for usage according to the business rules of the process.</t>
+  </si>
+  <si>
+    <t>This sheet is the place to store plain data, as well as most user data with the important exception of credential names.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typically there is not much for you to add here, although you want to check/change the settings of the Retry mechanism implemented in at the framework layer, during transaction processing, exception recovery, and continuous failiure. Also stores constants used throughout the program, like preconfiguered delays, timeouts. </t>
+  </si>
+  <si>
+    <t>This sheet is used to fetch assets from Orchestrator. The column name is the key, while the column asset hoolds the asset name in Orchestrator. If there is another local key with the same name, it will be overwritten by the value fetched from Orchestrator.</t>
+  </si>
+  <si>
+    <t>####  Legend of Key Value pair colours####</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -343,6 +391,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -422,7 +477,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -453,6 +508,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -773,15 +837,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="116.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="118" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
@@ -789,36 +853,119 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="7"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="9" t="s">
+    <row r="2" spans="1:1" ht="18.75">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:1" ht="60">
+      <c r="A3" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="30">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:1" ht="15.75">
+      <c r="A4" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75">
+      <c r="A6" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="45">
+      <c r="A7" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75">
+      <c r="A8" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75">
+      <c r="A10" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="30">
+      <c r="A11" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="45">
+      <c r="A12" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="45">
+      <c r="A13" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75">
+      <c r="A15" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="45">
+      <c r="A16" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75">
+      <c r="A17" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30">
+      <c r="A18" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="15"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="30">
+      <c r="A21" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="10" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="11" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="12" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="13" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" s="13" t="s">
         <v>78</v>
       </c>
     </row>
@@ -833,7 +980,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3066,7 +3213,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3163,7 +3310,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Moved the State machine around just to make the looks better. OrchestratorQueueName key from Config.xlsx used in the frameworklayer
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043FFA49-94A4-4929-93EF-C72B6878557D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAF80AD-4710-417F-8AE1-3E78E2E94A16}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -839,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -896,7 +896,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="30">
+    <row r="11" spans="1:1" ht="45">
       <c r="A11" s="15" t="s">
         <v>94</v>
       </c>
@@ -906,7 +906,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="45">
+    <row r="13" spans="1:1" ht="60">
       <c r="A13" s="15" t="s">
         <v>95</v>
       </c>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1070,7 +1070,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">

</xml_diff>

<commit_message>
Now calling GetDataTask outside GetSetTransactionData.xaml. fixed businessRuleException boolean flag to isBusinessRuleException. Usuing Orchestrator 2018 robot authentication for REST API
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAF80AD-4710-417F-8AE1-3E78E2E94A16}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20C2D0E-5FCD-462C-85FB-1392A51437A3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -101,24 +101,6 @@
   </si>
   <si>
     <t>Image accuracy high value, for images that have low contrast. Must be double</t>
-  </si>
-  <si>
-    <t>OrchestratorURL</t>
-  </si>
-  <si>
-    <t>The URL of your orchestrator server. This property is used only if you are using a Queue to store your Transaction Items.</t>
-  </si>
-  <si>
-    <t>OrchestratorCredentialName</t>
-  </si>
-  <si>
-    <t>The name of Orchestrator credentials. This should be stored in Windows Credential manager. This property is used only if you are using a Queue to store your Transaction Items.</t>
-  </si>
-  <si>
-    <t>OrchestratorTenancyName</t>
-  </si>
-  <si>
-    <t>The name of the Orchestrator tenant.  This property is used only if you are using a Queue to store your Transaction Items.</t>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
@@ -170,9 +152,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Enable the execution of the FirstRun Task. </t>
-  </si>
-  <si>
     <t>Task path location</t>
   </si>
   <si>
@@ -263,9 +242,6 @@
     <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
   </si>
   <si>
-    <t>This Key is used only during Debug. You can delete in production</t>
-  </si>
-  <si>
     <t>This key belongs to user designated category 1</t>
   </si>
   <si>
@@ -327,6 +303,12 @@
   </si>
   <si>
     <t>####  Legend of Key Value pair colours####</t>
+  </si>
+  <si>
+    <t>Enable the execution of the FirstRun Task. (0=disable, 1=enable)</t>
+  </si>
+  <si>
+    <t>This key belongs to user designated category 2</t>
   </si>
 </sst>
 </file>
@@ -352,13 +334,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -402,6 +377,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -417,17 +399,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -473,9 +455,9 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -488,44 +470,44 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -839,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -850,7 +832,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75">
@@ -858,115 +840,115 @@
     </row>
     <row r="3" spans="1:1" ht="60">
       <c r="A3" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75">
+      <c r="A4" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75">
+      <c r="A6" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="45">
+      <c r="A7" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75">
+      <c r="A8" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75">
-      <c r="A4" s="14" t="s">
+    <row r="10" spans="1:1" ht="15.75">
+      <c r="A10" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="45">
+      <c r="A11" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="45">
+      <c r="A12" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75">
-      <c r="A6" s="14" t="s">
+    <row r="13" spans="1:1" ht="60">
+      <c r="A13" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="45">
-      <c r="A7" s="15" t="s">
+    <row r="15" spans="1:1" ht="15.75">
+      <c r="A15" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="45">
+      <c r="A16" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75">
+      <c r="A17" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30">
+      <c r="A18" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75">
-      <c r="A8" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.75">
-      <c r="A10" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="45">
-      <c r="A11" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="45">
-      <c r="A12" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="60">
-      <c r="A13" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.75">
-      <c r="A15" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="45">
-      <c r="A16" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75">
-      <c r="A17" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="30">
-      <c r="A18" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="15"/>
+      <c r="A19" s="14"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="30">
-      <c r="A21" s="16" t="s">
-        <v>77</v>
+      <c r="A21" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="11" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="12" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="13" t="s">
-        <v>78</v>
+      <c r="A25" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -979,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1027,54 +1009,54 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
@@ -2061,10 +2043,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC672C-F735-4EF3-8287-9B35E6A7A36A}">
-  <dimension ref="A1:Z991"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2109,30 +2091,9 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
@@ -3103,9 +3064,6 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3139,68 +3097,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3213,7 +3171,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3236,68 +3194,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="b">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3363,29 +3321,29 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -4501,10 +4459,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>

<commit_message>
Workblocks now have a local Audit variable that collects child workblock information. Audit no longer bubbles up globally
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97AE96D-7AFD-43C7-9DC5-6517A7E3FB1E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1126EB74-3D7E-4FC0-A6F8-C28B47715B24}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>This key belongs to user designated category 2</t>
+  </si>
+  <si>
+    <t>KibanaDemoQueue</t>
   </si>
 </sst>
 </file>
@@ -962,7 +965,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1023,7 +1026,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -1054,6 +1057,9 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -3171,7 +3177,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3208,7 +3214,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>92</v>
@@ -3230,7 +3236,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Simplified workblock interface. All exceptions are now rethrown, so wbHandleExec no longer exists
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPath_REFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Documents\UiPath\new\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1126EB74-3D7E-4FC0-A6F8-C28B47715B24}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41824550-794F-4E48-8A5C-444ED25272E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -121,25 +121,10 @@
     <t>Description (Assets will always overwrite other config)</t>
   </si>
   <si>
-    <t>wbInit_Type</t>
-  </si>
-  <si>
     <t>wbGetTransactionData_Type</t>
   </si>
   <si>
     <t>wbProcessTransaction_Type</t>
-  </si>
-  <si>
-    <t>wbInit_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>wbGetTransactionData_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>wbProcessTransaction_SuppressSuccessful</t>
-  </si>
-  <si>
-    <t>Do not log successful executions of wb</t>
   </si>
   <si>
     <t>Name of Workblock</t>
@@ -312,6 +297,42 @@
   </si>
   <si>
     <t>KibanaDemoQueue</t>
+  </si>
+  <si>
+    <t>wbInitAllApplications_Type</t>
+  </si>
+  <si>
+    <t>wbCloseAllApplications_Type</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>SystemTask1_wbType</t>
+  </si>
+  <si>
+    <t>SystemTask2_wbType</t>
+  </si>
+  <si>
+    <t>Task1_Env</t>
+  </si>
+  <si>
+    <t>Task2_Env</t>
+  </si>
+  <si>
+    <t>Task1_wbType</t>
+  </si>
+  <si>
+    <t>Task2_wbType</t>
+  </si>
+  <si>
+    <t>FirstRunTask</t>
+  </si>
+  <si>
+    <t>GetDataTask</t>
+  </si>
+  <si>
+    <t>Name of task main workblock</t>
   </si>
 </sst>
 </file>
@@ -416,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -454,6 +475,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -462,13 +494,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -504,6 +533,8 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -834,124 +865,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18.75">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:1" ht="60">
+      <c r="A3" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75">
+      <c r="A4" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75">
+      <c r="A6" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="45">
+      <c r="A7" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75">
+      <c r="A8" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75">
+      <c r="A10" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75">
-      <c r="A2" s="8"/>
-    </row>
-    <row r="3" spans="1:1" ht="60">
-      <c r="A3" s="7" t="s">
+    <row r="11" spans="1:1" ht="45">
+      <c r="A11" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="45">
+      <c r="A12" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="60">
+      <c r="A13" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75">
+      <c r="A15" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75">
-      <c r="A4" s="13" t="s">
+    <row r="16" spans="1:1" ht="45">
+      <c r="A16" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75">
+      <c r="A17" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="14" t="s">
+    <row r="18" spans="1:1" ht="30">
+      <c r="A18" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="13"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="30">
+      <c r="A21" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="15" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75">
-      <c r="A6" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="45">
-      <c r="A7" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75">
-      <c r="A8" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.75">
-      <c r="A10" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="45">
-      <c r="A11" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="45">
-      <c r="A12" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="60">
-      <c r="A13" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.75">
-      <c r="A15" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="45">
-      <c r="A16" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75">
-      <c r="A17" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="30">
-      <c r="A18" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="14"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="30">
-      <c r="A21" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="16" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -964,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1011,62 +1042,62 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>54</v>
+      <c r="A3" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>55</v>
+      <c r="A4" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>67</v>
+      <c r="A5" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
@@ -3077,10 +3108,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3102,69 +3133,47 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="3" t="b">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="3" t="b">
-        <v>1</v>
+      <c r="A5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3174,15 +3183,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
   </cols>
@@ -3199,69 +3208,113 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
-        <v>43</v>
+      <c r="A2" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>48</v>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3320,40 +3373,40 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>53</v>
+      <c r="A3" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>63</v>
+      <c r="A4" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -3365,7 +3418,7 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7">
@@ -3376,7 +3429,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -3387,7 +3440,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -3399,7 +3452,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11">
@@ -3410,7 +3463,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12">
@@ -3421,7 +3474,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B13">
@@ -3433,7 +3486,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B15">
@@ -3444,7 +3497,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B16">
@@ -3455,7 +3508,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B17">

</xml_diff>

<commit_message>
Removed audit object. Framework now uses log field values to register progress
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,28 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Documents\UiPath\new\UiPath_REFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Documents\UiPath\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41824550-794F-4E48-8A5C-444ED25272E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23177095-A869-4757-ADB1-02498B8E3DB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
     <sheet name="Settings" sheetId="1" r:id="rId2"/>
     <sheet name="Credentials" sheetId="6" r:id="rId3"/>
-    <sheet name="Workblocks" sheetId="4" r:id="rId4"/>
-    <sheet name="Tasks" sheetId="5" r:id="rId5"/>
-    <sheet name="Constants" sheetId="2" r:id="rId6"/>
-    <sheet name="Assets" sheetId="3" r:id="rId7"/>
+    <sheet name="Tasks" sheetId="5" r:id="rId4"/>
+    <sheet name="Constants" sheetId="2" r:id="rId5"/>
+    <sheet name="Assets" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -119,15 +118,6 @@
   </si>
   <si>
     <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>wbGetTransactionData_Type</t>
-  </si>
-  <si>
-    <t>wbProcessTransaction_Type</t>
-  </si>
-  <si>
-    <t>Name of Workblock</t>
   </si>
   <si>
     <t>ServicesLayer\FirstRun\</t>
@@ -161,15 +151,9 @@
     <t>Enable Task setting. [0=Disable. 1=Enable during first run, 2=Always enable]</t>
   </si>
   <si>
-    <t>Task1</t>
-  </si>
-  <si>
     <t>ServicesLayer\Task1</t>
   </si>
   <si>
-    <t>Task2</t>
-  </si>
-  <si>
     <t>ServicesLayer\Task2</t>
   </si>
   <si>
@@ -191,15 +175,6 @@
     <t>Data\Output\</t>
   </si>
   <si>
-    <t>Init</t>
-  </si>
-  <si>
-    <t>GetData</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
     <t>REFrameWork</t>
   </si>
   <si>
@@ -248,9 +223,6 @@
     <t>Credentials</t>
   </si>
   <si>
-    <t>Workblocks</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -263,9 +235,6 @@
     <t>The credentials sheet is the place to store your credential names.There is also one special credential, that needs to be defined only once, and which is comprised of the URL, TenancyName and CredentialName required to authenticate to the Orchestrator server using REST API. This is only used when working with QueueItems.</t>
   </si>
   <si>
-    <t>The workblock names are of the states in the framework. Define the names of workblocks you create here.</t>
-  </si>
-  <si>
     <t>FirstRunTask: This task is invoked in the Framework Layer and executes only once(Even if Transaction number 1 were to fail and be retried, it would not be executed again), at program startup. It should not interact with data in memory, since it executes before we enter the main process data layer, but it can be used as a queue dispatcher.</t>
   </si>
   <si>
@@ -299,40 +268,10 @@
     <t>KibanaDemoQueue</t>
   </si>
   <si>
-    <t>wbInitAllApplications_Type</t>
-  </si>
-  <si>
-    <t>wbCloseAllApplications_Type</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>SystemTask1_wbType</t>
-  </si>
-  <si>
-    <t>SystemTask2_wbType</t>
-  </si>
-  <si>
     <t>Task1_Env</t>
   </si>
   <si>
     <t>Task2_Env</t>
-  </si>
-  <si>
-    <t>Task1_wbType</t>
-  </si>
-  <si>
-    <t>Task2_wbType</t>
-  </si>
-  <si>
-    <t>FirstRunTask</t>
-  </si>
-  <si>
-    <t>GetDataTask</t>
-  </si>
-  <si>
-    <t>Name of task main workblock</t>
   </si>
 </sst>
 </file>
@@ -437,7 +376,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -475,17 +414,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -494,7 +422,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -533,7 +461,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -853,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -866,7 +793,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75">
@@ -874,115 +801,105 @@
     </row>
     <row r="3" spans="1:1" ht="60">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="13" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="12" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="45">
       <c r="A7" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" ht="45">
       <c r="A9" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:1" ht="45">
+      <c r="A10" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="60">
+      <c r="A11" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75">
+      <c r="A13" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="45">
+      <c r="A14" s="13" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="45">
-      <c r="A11" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="45">
-      <c r="A12" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="60">
-      <c r="A13" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="30">
+      <c r="A16" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="45">
-      <c r="A16" s="13" t="s">
-        <v>84</v>
-      </c>
+    <row r="17" spans="1:1">
+      <c r="A17" s="13"/>
     </row>
-    <row r="17" spans="1:1" ht="15.75">
-      <c r="A17" s="12" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="30">
-      <c r="A18" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="13"/>
+    <row r="19" spans="1:1" ht="30">
+      <c r="A19" s="14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="8" t="s">
-        <v>86</v>
+      <c r="A20" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="30">
-      <c r="A21" s="14" t="s">
-        <v>65</v>
+    <row r="21" spans="1:1">
+      <c r="A21" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="9" t="s">
-        <v>67</v>
+      <c r="A22" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="15" t="s">
-        <v>88</v>
+      <c r="A23" s="15" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1046,7 +963,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1054,35 +971,35 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1090,7 +1007,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -3107,86 +3024,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B87B5F-FB11-4C00-9666-7AE89EF4CC06}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3209,112 +3051,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>87</v>
+      <c r="C4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>43</v>
+      <c r="C7" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
+    <row r="8" spans="1:3">
+      <c r="A8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3322,7 +3120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
@@ -3380,29 +3178,29 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -4502,7 +4300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>

</xml_diff>

<commit_message>
Change log message level to error from info when workblock failed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Documents\UiPath\UiPath_REFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Documents\UiPath\UiPath Enchanced REFramework\UiPath_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23177095-A869-4757-ADB1-02498B8E3DB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D57E58-D9F6-4442-80F4-AECB8ADA93C6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
-  </si>
-  <si>
-    <t>wbBusinessProcessName</t>
-  </si>
-  <si>
-    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
     <t>Asset</t>
@@ -160,24 +154,6 @@
     <t>MaxInitRetryNumber</t>
   </si>
   <si>
-    <t>Debug_wbSaveReport</t>
-  </si>
-  <si>
-    <t>Debug_wbSaveReportPath</t>
-  </si>
-  <si>
-    <t>Set to TRUE to enable storage of each application run. It contains a detailed report, per Workblock executed</t>
-  </si>
-  <si>
-    <t>Path to save the reports. Relative or absolute</t>
-  </si>
-  <si>
-    <t>Data\Output\</t>
-  </si>
-  <si>
-    <t>REFrameWork</t>
-  </si>
-  <si>
     <t>MaxContinuousRetryNumber</t>
   </si>
   <si>
@@ -188,15 +164,6 @@
   </si>
   <si>
     <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
-  </si>
-  <si>
-    <t>Debug_wbFileFormat</t>
-  </si>
-  <si>
-    <t>Options are csv and json. Default option is csv</t>
-  </si>
-  <si>
-    <t>csv</t>
   </si>
   <si>
     <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
@@ -782,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -793,7 +760,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="7" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75">
@@ -801,72 +768,72 @@
     </row>
     <row r="3" spans="1:1" ht="60">
       <c r="A3" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="13" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="45">
       <c r="A7" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="12" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="45">
       <c r="A9" s="13" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="45">
       <c r="A10" s="13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="60">
       <c r="A11" s="13" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="45">
       <c r="A14" s="13" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30">
       <c r="A16" s="13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -874,32 +841,32 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="8" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="30">
       <c r="A19" s="14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="10" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="11" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="15" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -960,62 +927,23 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
-      <c r="B8" s="3"/>
-    </row>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
     <row r="26" ht="14.25" customHeight="1"/>
@@ -1984,11 +1912,6 @@
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3051,68 +2974,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3178,29 +3101,29 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -4316,10 +4239,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>